<commit_message>
output old data new classifier
</commit_message>
<xml_diff>
--- a/Kfolds/Kfold_results_SD.xlsx
+++ b/Kfolds/Kfold_results_SD.xlsx
@@ -10,6 +10,7 @@
     <sheet name="medbert" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="pubmed_fulltext" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="basebert" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="basebert1" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1349,4 +1350,314 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fold</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Epoch</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Fbeta</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Best Recall</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Best Precision</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Best Threshold</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>False Neg(0.5)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>False Pos(0.5)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Val loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fold_0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>18.09_09.50</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.71794873</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.23140496</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.82038</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.50541514</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>22</v>
+      </c>
+      <c r="M2" t="n">
+        <v>186</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.5986553269128004</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fold_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>18.09_10.00</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.8076923</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.23684211</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.8117444</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.5449827</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>15</v>
+      </c>
+      <c r="M3" t="n">
+        <v>203</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.7180119156837463</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fold_2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>18.09_10.12</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.8717949</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.32380953</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.8687392</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.651341</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M4" t="n">
+        <v>142</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.8751945644617081</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fold_3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18.09_10.25</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.8101266</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.24521072</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.8169257</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.5545927</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15</v>
+      </c>
+      <c r="M5" t="n">
+        <v>197</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.8309154734015465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
output medbert new data
</commit_message>
<xml_diff>
--- a/Kfolds/Kfold_results_SD.xlsx
+++ b/Kfolds/Kfold_results_SD.xlsx
@@ -11,6 +11,7 @@
     <sheet name="pubmed_fulltext" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="basebert" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="basebert1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="medbert1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1660,4 +1661,314 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fold</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Epoch</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Fbeta</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Best Recall</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Best Precision</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Best Threshold</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>False Neg(0.5)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>False Pos(0.5)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Val loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fold_0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>18.09_11.56</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.64935064</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.28089887</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.8647469</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.5144033</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>27</v>
+      </c>
+      <c r="M2" t="n">
+        <v>128</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.6564610414206982</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fold_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>18.09_12.10</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.8051948</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.31958762</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.87172776</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.61752987</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>15</v>
+      </c>
+      <c r="M3" t="n">
+        <v>132</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.5011956257124742</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fold_2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>18.09_12.24</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.8831169</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.3090909</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.8595113</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.6439394</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.961</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.2298</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2207</v>
+      </c>
+      <c r="L4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M4" t="n">
+        <v>152</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.4681512216726939</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fold_3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18.09_12.38</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.8717949</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.272</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.83246076</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.6049822</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>10</v>
+      </c>
+      <c r="M5" t="n">
+        <v>182</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.5822798783580462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
output medbert10 balanced data
</commit_message>
<xml_diff>
--- a/Kfolds/Kfold_results_SD.xlsx
+++ b/Kfolds/Kfold_results_SD.xlsx
@@ -12,6 +12,7 @@
     <sheet name="basebert" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="basebert1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="medbert1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="medbert2" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1971,4 +1972,314 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fold</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Epoch</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Fbeta</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Best Recall</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Best Precision</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Best Threshold</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>False Neg(0.5)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>False Pos(0.5)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Val loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fold_0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>19.09_09.08</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.6363636</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.35766423</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.8987784</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.5505618</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>28</v>
+      </c>
+      <c r="M2" t="n">
+        <v>88</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.7052134337524573</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fold_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>19.09_09.15</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.7922078</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.36746988</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.8944154</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.6434599</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>16</v>
+      </c>
+      <c r="M3" t="n">
+        <v>105</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.3302207328379154</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fold_2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19.09_09.23</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.8701299</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.34358975</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.87958115</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.666004</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M4" t="n">
+        <v>128</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.7126566295822462</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fold_3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>19.09_09.30</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.7948718</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.3668639</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.89267015</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.64449066</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M5" t="n">
+        <v>107</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.3642424587160349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
output pubmed_fulltext higher lr
</commit_message>
<xml_diff>
--- a/Kfolds/Kfold_results_SD.xlsx
+++ b/Kfolds/Kfold_results_SD.xlsx
@@ -14,6 +14,7 @@
     <sheet name="pubmed_fulltext" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="basebert" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="pubmed_fulltext1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="pubmed_fulltext2" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2593,4 +2594,314 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fold</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Epoch</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Fbeta</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Best Recall</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Best Precision</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Best Threshold</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>False Neg(0.5)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>False Pos(0.5)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Val loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fold_0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>13.10_09.26</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.8467742</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.41501975</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.86510503</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.7009346</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>19</v>
+      </c>
+      <c r="M2" t="n">
+        <v>148</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.6406238003964385</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fold_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>13.10_09.41</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.42910448</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.868336</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.74869794</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.968</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4158</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.2996</v>
+      </c>
+      <c r="L3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" t="n">
+        <v>153</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.7133551667774877</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fold_2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>13.10_09.58</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.928</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.4566929</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.8812601</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.7692308</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.1213</v>
+      </c>
+      <c r="L4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M4" t="n">
+        <v>138</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.5740149182177359</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fold_3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>13.10_10.16</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.944</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.43223444</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.8691438</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.76326</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.4364</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.4906</v>
+      </c>
+      <c r="L5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M5" t="n">
+        <v>155</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.5730994257234758</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>